<commit_message>
Updated with Git mail sequence
</commit_message>
<xml_diff>
--- a/InsuranceClaimAutomation - UiPATH/query1.xlsx
+++ b/InsuranceClaimAutomation - UiPATH/query1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -48,9 +48,6 @@
     <t>SUM INSURED</t>
   </si>
   <si>
-    <t>CLAIM AMOUNT</t>
-  </si>
-  <si>
     <t>NCB &lt; 3</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Claim Amount</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -324,22 +318,25 @@
     <t>Minor</t>
   </si>
   <si>
+    <t>Declined</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Workshop AMT</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
     <t>Duplicate</t>
-  </si>
-  <si>
-    <t>Verified</t>
-  </si>
-  <si>
-    <t>Declined</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -705,7 +702,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K8"/>
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,22 +728,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" t="s">
-        <v>71</v>
-      </c>
       <c r="J1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -763,22 +760,22 @@
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F2">
         <v>10000</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>2016</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -795,22 +792,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3">
         <v>25000</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3">
         <v>2015</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -827,22 +824,22 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F4">
         <v>10000</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4">
         <v>2016</v>
       </c>
       <c r="J4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -859,22 +856,22 @@
         <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5">
         <v>2017</v>
       </c>
       <c r="J5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -891,22 +888,22 @@
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6">
         <v>18000</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6">
         <v>2010</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -923,22 +920,22 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7">
         <v>20000</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7">
         <v>2013</v>
       </c>
       <c r="J7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -955,22 +952,22 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8">
         <v>20000</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8">
         <v>2018</v>
       </c>
       <c r="J8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1008,16 +1005,16 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1040,10 +1037,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -1072,10 +1069,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -1104,10 +1101,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -1137,10 +1134,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -1169,10 +1166,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -1198,10 +1195,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -1241,22 +1238,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1273,10 +1270,10 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1293,10 +1290,10 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1313,10 +1310,10 @@
         <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1333,10 +1330,10 @@
         <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1362,24 +1359,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>2014</v>
@@ -1390,10 +1387,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>2015</v>
@@ -1404,10 +1401,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>2016</v>
@@ -1418,10 +1415,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>2017</v>
@@ -1432,10 +1429,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>2015</v>
@@ -1446,10 +1443,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>2016</v>
@@ -1460,10 +1457,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>2017</v>
@@ -1474,10 +1471,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>2015</v>
@@ -1488,10 +1485,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>2016</v>
@@ -1502,10 +1499,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>2017</v>
@@ -1516,10 +1513,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>2015</v>
@@ -1530,10 +1527,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>2016</v>
@@ -1544,10 +1541,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>2017</v>
@@ -1558,10 +1555,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>1994</v>
@@ -1572,10 +1569,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>1995</v>
@@ -1587,10 +1584,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>1996</v>
@@ -1602,10 +1599,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1997</v>
@@ -1617,10 +1614,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>1998</v>
@@ -1632,10 +1629,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>1999</v>
@@ -1647,10 +1644,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21">
         <v>2000</v>
@@ -1662,10 +1659,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>2001</v>
@@ -1677,10 +1674,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>2002</v>
@@ -1692,10 +1689,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>2003</v>
@@ -1707,10 +1704,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>2004</v>
@@ -1722,10 +1719,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>2005</v>
@@ -1737,10 +1734,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>2006</v>
@@ -1752,10 +1749,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>2007</v>
@@ -1767,10 +1764,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>2008</v>
@@ -1782,10 +1779,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>2009</v>
@@ -1797,10 +1794,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>2010</v>
@@ -1812,10 +1809,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32">
         <v>2011</v>
@@ -1827,10 +1824,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>2009</v>
@@ -1841,10 +1838,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34">
         <v>2010</v>
@@ -1855,10 +1852,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35">
         <v>2011</v>
@@ -1869,10 +1866,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36">
         <v>2012</v>
@@ -1883,10 +1880,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37">
         <v>2014</v>
@@ -1897,10 +1894,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38">
         <v>2010</v>
@@ -1911,10 +1908,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39">
         <v>2011</v>
@@ -1926,10 +1923,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40">
         <v>2012</v>
@@ -1941,10 +1938,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41">
         <v>2013</v>
@@ -1956,10 +1953,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42">
         <v>2014</v>
@@ -1971,10 +1968,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43">
         <v>2015</v>
@@ -1986,10 +1983,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C44">
         <v>2016</v>
@@ -2001,10 +1998,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C45">
         <v>2014</v>
@@ -2015,10 +2012,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46">
         <v>2015</v>
@@ -2030,10 +2027,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47">
         <v>2016</v>
@@ -2045,10 +2042,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48">
         <v>2017</v>
@@ -2060,10 +2057,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C49">
         <v>2018</v>
@@ -2090,340 +2087,340 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2446,25 +2443,25 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
       <c r="H1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2475,10 +2472,10 @@
         <v>10000000</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>2015</v>
@@ -2487,7 +2484,7 @@
         <v>1452000</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2498,10 +2495,10 @@
         <v>100000</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>2017</v>
@@ -2510,7 +2507,7 @@
         <v>1008000</v>
       </c>
       <c r="G3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H3">
         <v>121000</v>
@@ -2524,10 +2521,10 @@
         <v>500000</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>2018</v>
@@ -2536,7 +2533,7 @@
         <v>704000</v>
       </c>
       <c r="G4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H4">
         <v>550000</v>

</xml_diff>